<commit_message>
Statistics in R: Added Wilcoxon and permutation tests, solved package conflicts issue. Split in two documents: a working one to add new functions (working version) and a presentation one separating statistical analysis per POI
</commit_message>
<xml_diff>
--- a/analysis_progress.xlsx
+++ b/analysis_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentine\Documents\Scripts\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1295B77-AFC5-4B2A-834C-EBC99934289E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E994072-293F-4A45-BBCA-B0053BCE0E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plus" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="48">
   <si>
     <t>h+</t>
   </si>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1396,7 +1396,9 @@
       <c r="D13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -1406,8 +1408,12 @@
       <c r="J13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
+      <c r="K13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="O13" s="28"/>
@@ -1847,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F45A5A1-0549-409D-87A5-AA4A2734AB5E}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates: Aesthetic average plot (time), total plot dist (dPM) and POI progress table
</commit_message>
<xml_diff>
--- a/analysis_progress.xlsx
+++ b/analysis_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentine\Documents\Scripts\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E994072-293F-4A45-BBCA-B0053BCE0E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C442E76-0999-4213-8DA0-CB0AA81BDC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="48">
   <si>
     <t>h+</t>
   </si>
@@ -745,7 +745,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1399,8 +1399,12 @@
       <c r="E13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="F13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="17"/>
       <c r="I13" s="12" t="s">
         <v>26</v>
@@ -1414,7 +1418,9 @@
       <c r="L13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="12"/>
+      <c r="M13" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="N13" s="12"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>

</xml_diff>

<commit_message>
Working version of all code updated to include another POI, Stats analysis on fusion marker file and update progress list
</commit_message>
<xml_diff>
--- a/analysis_progress.xlsx
+++ b/analysis_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentine\Documents\Scripts\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C442E76-0999-4213-8DA0-CB0AA81BDC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CFDEF6-FBED-44E1-8FEC-856043A79A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="48">
   <si>
     <t>h+</t>
   </si>
@@ -745,7 +745,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,7 +1353,9 @@
       <c r="G12" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="I12" s="10" t="s">
         <v>26</v>
       </c>
@@ -1369,7 +1371,9 @@
       <c r="M12" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N12" s="10"/>
+      <c r="N12" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
@@ -1405,7 +1409,9 @@
       <c r="G13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="I13" s="12" t="s">
         <v>26</v>
       </c>
@@ -1421,7 +1427,9 @@
       <c r="M13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="12"/>
+      <c r="N13" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="28"/>

</xml_diff>

<commit_message>
modifications plots to add CRIB and Ste4
</commit_message>
<xml_diff>
--- a/analysis_progress.xlsx
+++ b/analysis_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentine\Documents\Scripts\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CFDEF6-FBED-44E1-8FEC-856043A79A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4E00C7-4530-4470-8851-539D28801AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plus" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="56">
   <si>
     <t>h+</t>
   </si>
@@ -177,6 +177,30 @@
   </si>
   <si>
     <t>not needed</t>
+  </si>
+  <si>
+    <t>change this column by the strain name</t>
+  </si>
+  <si>
+    <t>yvt225</t>
+  </si>
+  <si>
+    <t>yvt239</t>
+  </si>
+  <si>
+    <t>yvt196</t>
+  </si>
+  <si>
+    <t>yvt98</t>
+  </si>
+  <si>
+    <t>yvt198</t>
+  </si>
+  <si>
+    <t>yvt86</t>
+  </si>
+  <si>
+    <t>yvt77</t>
   </si>
 </sst>
 </file>
@@ -742,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1272,7 +1296,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>26</v>
@@ -1336,7 +1360,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>26</v>
@@ -1392,7 +1416,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>26</v>
@@ -1604,7 +1628,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>26</v>
@@ -1664,7 +1688,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>26</v>
@@ -1809,7 +1833,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>26</v>
@@ -1852,6 +1876,11 @@
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
     </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="I1:N1"/>
@@ -1867,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F45A5A1-0549-409D-87A5-AA4A2734AB5E}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2152,7 +2181,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>26</v>

</xml_diff>